<commit_message>
[master]finished php tutorial1 and 2 update
</commit_message>
<xml_diff>
--- a/tutorials/tutorial_01/review_points_WaiLinOo.xlsx
+++ b/tutorials/tutorial_01/review_points_WaiLinOo.xlsx
@@ -92,7 +92,7 @@
 2) Star must be displayed in 1,3,5,7,9,11,9,7,5,3,1 pattern</t>
   </si>
   <si>
-    <t>Done</t>
+    <t>Done pattern</t>
   </si>
   <si>
     <t>エラータイプ</t>
@@ -130,10 +130,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -149,30 +149,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,16 +164,38 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,41 +208,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,15 +232,47 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,7 +287,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,181 +333,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,15 +644,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -688,26 +661,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,153 +706,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1986,10 +1968,10 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="P3" sqref="P3:U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="5.44166666666667" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.1083333333333" style="3" customWidth="1"/>

</xml_diff>